<commit_message>
Update Provenance. Switch Version to 0.1.12 Add Provenance Examples for Transmitter, Author-Organization, Author-Practitioner and Source-Payer. Updated PDexProvenance.md Page Changed Valueset names Extended Codeset for ConversionSource
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-ProvenanceConversionFrom.xlsx
+++ b/output/StructureDefinition-ProvenanceConversionFrom.xlsx
@@ -270,10 +270,10 @@
     <t>extensible</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/ValueSet-ProvenanceFormatConversionSourceVS</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-pdex/ImplementationGuide/davinci-pdex/StructureDefinition/ProvenanceConversionFrom</t>
+    <t>http://hl7.org/fhir/us/davinci-pdex/ValueSet/ProvenancePayerConversionSource</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-pdex/StructureDefinition/ProvenanceConversionFrom</t>
   </si>
   <si>
     <t>base64Binary
@@ -459,7 +459,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="19.796875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="74.8203125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="78.5703125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="43.0625" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Add CARIN/PDex background to index.md Add CARIN/PDex diagram Update version 0.1.17
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-ProvenanceConversionFrom.xlsx
+++ b/output/StructureDefinition-ProvenanceConversionFrom.xlsx
@@ -245,7 +245,7 @@
     <t>extensible</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-pdex/ValueSet/ProvenancePayerConversionSource</t>
+    <t>http://hl7.org/fhir/us/davinci-pdex/ValueSet/ProvenancePayerSourceFormat</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="19.796875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="78.5703125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="74.5390625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="43.0625" customWidth="true" bestFit="true"/>

</xml_diff>